<commit_message>
JCSantos - Casi OK. Antes de informe
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1746697622" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1746697622" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1746697622" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1746697622"/>
+      <pm:revision xmlns:pm="smNativeData" day="1746706751" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1746706751" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1746706751" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1746706751"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -105,6 +105,12 @@
     <t>Extra\cuerpo2.html</t>
   </si>
   <si>
+    <t>CorreoHtmlSinElementos</t>
+  </si>
+  <si>
+    <t>Extra\cuerpo3.html</t>
+  </si>
+  <si>
     <t>CorreoHtmlOK</t>
   </si>
   <si>
@@ -121,6 +127,12 @@
   </si>
   <si>
     <t>Respuesta a consulta sobre libros</t>
+  </si>
+  <si>
+    <t>AsuntoSinTransacciones</t>
+  </si>
+  <si>
+    <t>Sin correos que procesar</t>
   </si>
   <si>
     <t>MaxRetryNumber</t>
@@ -247,7 +259,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1746697622" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1746706751" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -262,7 +274,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1746697622" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1746706751" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -278,7 +290,7 @@
       <sz val="14"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1746697622" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1746706751" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="280" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="280" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="280" lang="default" weight="bold"/>
@@ -300,7 +312,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1746697622" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1746706751" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -322,7 +334,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1746697622"/>
+          <pm:border xmlns:pm="smNativeData" id="1746706751"/>
         </ext>
       </extLst>
     </border>
@@ -341,7 +353,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1746697622"/>
+          <pm:border xmlns:pm="smNativeData" id="1746706751"/>
         </ext>
       </extLst>
     </border>
@@ -362,10 +374,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1746697622" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1746706751" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1746697622" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1746706751" count="2">
         <pm:color name="Color 25" rgb="D69D85"/>
         <pm:color name="Color 24" rgb="C8C8C8"/>
       </pm:colors>
@@ -630,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="13" defaultColWidth="14.428571" defaultRowHeight="15" customHeight="1"/>
@@ -795,8 +807,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="21" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:1" ht="14.25" customHeight="1"/>
@@ -1777,11 +1803,12 @@
     <row r="998" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="999" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="1000" spans="1:1" ht="14.25" customHeight="1"/>
+    <row r="1001" spans="1:1" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1746697622" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1746706751" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1790,16 +1817,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746697622" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746706751" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1860,138 +1887,138 @@
     </row>
     <row r="2" spans="1:3" ht="15.40">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.40">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:3" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:3" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="15.40">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.25" customHeight="1"/>
@@ -2969,7 +2996,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1746697622" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1746706751" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2978,16 +3005,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746697622" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746706751" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3017,13 +3044,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -4051,7 +4078,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1746697622" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1746706751" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4060,16 +4087,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1746697622" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1746697622" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1746706751" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1746706751" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746697622" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1746706751" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>